<commit_message>
Advanced Digital Design Project
</commit_message>
<xml_diff>
--- a/UCSD_ECE111/project_4_1/summary.xlsx
+++ b/UCSD_ECE111/project_4_1/summary.xlsx
@@ -28,9 +28,6 @@
     <t>SectionId</t>
   </si>
   <si>
-    <t>#ALUTs</t>
-  </si>
-  <si>
     <t>#Registers</t>
   </si>
   <si>
@@ -88,6 +85,10 @@
   </si>
   <si>
     <t>performance</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ALUTs</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
@@ -1006,7 +1007,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,61 +1039,61 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6">
         <v>937298</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="6">
-        <v>2129</v>
+        <v>2140</v>
       </c>
       <c r="H2" s="6">
         <v>1663</v>
       </c>
       <c r="I2" s="9">
         <f>G2+H2</f>
-        <v>3792</v>
+        <v>3803</v>
       </c>
       <c r="J2" s="6">
         <v>192.2</v>
@@ -1106,37 +1107,37 @@
       </c>
       <c r="M2" s="10">
         <f>I2*L2/1000</f>
-        <v>44.628012486992716</v>
+        <v>44.757471383975023</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="6">
         <v>937300</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" s="6">
-        <v>2129</v>
+        <v>2140</v>
       </c>
       <c r="H3" s="6">
         <v>1663</v>
       </c>
       <c r="I3" s="9">
         <f>G3+H3</f>
-        <v>3792</v>
+        <v>3803</v>
       </c>
       <c r="J3" s="6">
         <v>192.2</v>
@@ -1150,7 +1151,7 @@
       </c>
       <c r="M3" s="10">
         <f>I3*L3/1000</f>
-        <v>44.628012486992716</v>
+        <v>44.757471383975023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>